<commit_message>
Added DB dependencies in pom .xml
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="5175" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="5175" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId1"/>
     <sheet name="UserDetails" sheetId="2" r:id="rId2"/>
     <sheet name="Users" sheetId="4" r:id="rId3"/>
     <sheet name="SignUpUserDetails" sheetId="5" r:id="rId4"/>
-    <sheet name="Login" sheetId="3" r:id="rId5"/>
+    <sheet name="Enroll" sheetId="6" r:id="rId5"/>
+    <sheet name="Login1" sheetId="3" r:id="rId6"/>
+    <sheet name="Login" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J15"/>
+  <oleSize ref="A1:O15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -243,6 +245,15 @@
   </si>
   <si>
     <t>admin1@email.com</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>admin@email.com</t>
   </si>
 </sst>
 </file>
@@ -677,7 +688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="409.6">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -685,7 +696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="409.6">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -693,7 +704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="409.6">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -704,7 +715,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="409.6">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1016,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1043,7 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1113,10 +1124,49 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:I17"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1224,4 +1274,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified pages and testcases
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -3,20 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\com.learnautomation.hybrid\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="5175" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="5175" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId1"/>
     <sheet name="UserDetails" sheetId="2" r:id="rId2"/>
     <sheet name="Users" sheetId="4" r:id="rId3"/>
-    <sheet name="SignUpUserDetails" sheetId="5" r:id="rId4"/>
-    <sheet name="Enroll" sheetId="6" r:id="rId5"/>
-    <sheet name="Login1" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="10" r:id="rId4"/>
+    <sheet name="SignUpUserDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="CourseEnroll" sheetId="6" r:id="rId6"/>
     <sheet name="Login" sheetId="7" r:id="rId7"/>
+    <sheet name="CourseDetails" sheetId="8" r:id="rId8"/>
+    <sheet name="Category" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -115,33 +121,6 @@
     <t>Cypress</t>
   </si>
   <si>
-    <t>tutfu</t>
-  </si>
-  <si>
-    <t>ujtfurtur</t>
-  </si>
-  <si>
-    <t>tuut</t>
-  </si>
-  <si>
-    <t>tyujy</t>
-  </si>
-  <si>
-    <t>ytu</t>
-  </si>
-  <si>
-    <t>utytuyt</t>
-  </si>
-  <si>
-    <t>tytyytity</t>
-  </si>
-  <si>
-    <t>yiytity</t>
-  </si>
-  <si>
-    <t>tyityi</t>
-  </si>
-  <si>
     <t>Prashant</t>
   </si>
   <si>
@@ -244,9 +223,6 @@
     <t>nilamtest@gmail.com</t>
   </si>
   <si>
-    <t>admin1@email.com</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -254,6 +230,39 @@
   </si>
   <si>
     <t>admin@email.com</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>instructor</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>categoryName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">courseName </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation Testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Automation </t>
+  </si>
+  <si>
+    <t>This is test course</t>
+  </si>
+  <si>
+    <t>UI Automation</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Pune</t>
   </si>
 </sst>
 </file>
@@ -723,7 +732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="409.6">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -731,7 +740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="409.6">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -739,7 +748,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="19.5">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -747,7 +756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="409.6">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -755,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="409.6">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -763,7 +772,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="409.6">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -806,13 +815,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -829,13 +838,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>26</v>
@@ -852,13 +861,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>27</v>
@@ -875,13 +884,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>23</v>
@@ -893,18 +902,18 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>28</v>
@@ -921,16 +930,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -944,13 +953,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>27</v>
@@ -962,7 +971,7 @@
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1016,7 +1025,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1027,18 +1036,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1051,6 +1060,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1069,25 +1090,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1095,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -1122,12 +1143,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1138,140 +1159,24 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9975076028</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" display="admin1@email.com"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1280,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1292,18 +1197,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1313,4 +1218,88 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>